<commit_message>
Escribir nuevo produco realizado
</commit_message>
<xml_diff>
--- a/db/producto.xlsx
+++ b/db/producto.xlsx
@@ -1,78 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82572D3-E38F-49E0-B3F8-6289EA6703CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Productos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Uid</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Image</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Discount_price</t>
-  </si>
-  <si>
-    <t>IsActive</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Items</t>
-  </si>
-  <si>
-    <t>Pizza</t>
-  </si>
-  <si>
-    <t>Pizza familiar</t>
-  </si>
-  <si>
-    <t>[{"Name": "Queso", "amount": "1"}, {"Name": "Jam\u00f3n", "amount": "2"}]</t>
-  </si>
-  <si>
-    <t>pizza.jpg</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -87,7 +52,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -95,49 +60,23 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -179,7 +118,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -212,26 +151,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -264,23 +186,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -315,20 +220,16 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -450,56 +351,92 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Uid</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Image</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Price</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Discount_price</v>
+      </c>
+      <c r="F1" t="str">
+        <v>IsActive</v>
+      </c>
+      <c r="G1" t="str">
+        <v>Description</v>
+      </c>
+      <c r="H1" t="str">
+        <v>Items</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
+      <c r="B2" t="str">
+        <v>Pizza</v>
+      </c>
+      <c r="C2" t="str">
+        <v>pizza.jpg</v>
       </c>
       <c r="D2">
         <v>30000</v>
@@ -510,14 +447,42 @@
       <c r="F2" t="b">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
+      <c r="G2" t="str">
+        <v>Pizza familiar</v>
+      </c>
+      <c r="H2" t="str">
+        <v>[{"Name": "Queso", "amount": "1"}, {"Name": "Jam\u00f3n", "amount": "2"}]</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Pizza</v>
+      </c>
+      <c r="C3" t="str">
+        <v>pizza.jpg</v>
+      </c>
+      <c r="D3">
+        <v>30000</v>
+      </c>
+      <c r="E3">
+        <v>25000</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="str">
+        <v>Pizza familiar</v>
+      </c>
+      <c r="H3" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H3"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>